<commit_message>
filters cloned repos and gets similarity indexes from input git diff
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandra.veizu\Documents\Reframework_update_UiPath_Services\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0346df80bcaed32e/Desktop/Training/ProjectPlagiarismBot/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{9BE7DFF5-5AFC-4110-8461-609B0BDD5551}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8E12627C-F189-40D5-B40B-B61497D5502C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10" yWindow="40" windowWidth="10160" windowHeight="9340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -122,6 +122,18 @@
   </si>
   <si>
     <t>OrchestratorAssetFolder</t>
+  </si>
+  <si>
+    <t>ClonedRepoFilePath</t>
+  </si>
+  <si>
+    <t>C:\Users\nfh22\OneDrive\Desktop\Training\ProjectPlagiarismBot\Data\FilteredClones\</t>
+  </si>
+  <si>
+    <t>FilteredRepoFilePath</t>
+  </si>
+  <si>
+    <t>C:\Users\nfh22\OneDrive\Desktop\Training\ProjectPlagiarismBot\Data\Clones\</t>
   </si>
 </sst>
 </file>
@@ -499,16 +511,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -557,7 +569,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="30">
+    <row r="4" spans="1:26" ht="29">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -569,8 +581,22 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1574,12 +1600,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1616,7 +1642,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2682,16 +2708,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="30.1796875" customWidth="1"/>
+    <col min="3" max="3" width="60.26953125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Add GitCloneRepoFolderPath to Config.XLSX
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0346df80bcaed32e/Desktop/Training/ProjectPlagiarismBot/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\GitHub\uipath-automation-4\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{3CB869D0-AEA8-4759-AA46-C80BDBC3C72B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9C8A8000-7590-4FC9-8900-700ED46ABBAC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29B120A-25C0-418B-8A08-802FB2738B63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8040" yWindow="250" windowWidth="9510" windowHeight="9470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Name</t>
   </si>
@@ -151,40 +151,22 @@
     <t>Status message for TransactionData to record pending transaction.</t>
   </si>
   <si>
-    <t>InputCSVFilePath</t>
-  </si>
-  <si>
-    <t>Data\Input\GitHubRepoURLInput.csv</t>
-  </si>
-  <si>
-    <t>A relative path pointing to a place to look for the input CSV file before asking the user for input.</t>
-  </si>
-  <si>
-    <t>GitCloneRepoATargetPath</t>
-  </si>
-  <si>
-    <t>Data\Temp\RepoA</t>
-  </si>
-  <si>
-    <t>A relative path pointing to a place to clone the first repo in each transaction to be compared.</t>
-  </si>
-  <si>
-    <t>GitCloneRepoBTargetPath</t>
-  </si>
-  <si>
-    <t>Data\Temp\RepoB</t>
-  </si>
-  <si>
-    <t>A relative path pointing to a place to clone thesecond repo in each transaction to be compared.</t>
-  </si>
-  <si>
     <t>GitDiffOutputFolderPath</t>
   </si>
   <si>
     <t>Data\Temp\</t>
   </si>
   <si>
-    <t>A relative path pointing to a place to store the diff outputs for the repositories to be compared.</t>
+    <t>GitCloneRepoFolderPath</t>
+  </si>
+  <si>
+    <t>Data\Temp\RepoCloning</t>
+  </si>
+  <si>
+    <t>Folder path to Git Clone repo</t>
+  </si>
+  <si>
+    <t>Folder path to store Git Diff output .TXT file</t>
   </si>
 </sst>
 </file>
@@ -561,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z997"/>
+  <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -635,48 +617,28 @@
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:26" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A7" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:26" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" s="5" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A9" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1663,8 +1625,6 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add OutputMatrixFilePath to Config.XLSX
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\GitHub\uipath-automation-4\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F29B120A-25C0-418B-8A08-802FB2738B63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCFAC4F-F994-400A-A2F7-2564C4B772EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>Name</t>
   </si>
@@ -167,6 +167,15 @@
   </si>
   <si>
     <t>Folder path to store Git Diff output .TXT file</t>
+  </si>
+  <si>
+    <t>OutputMatrixFilePath</t>
+  </si>
+  <si>
+    <t>Data\Output\OutputMatrix.XLSX</t>
+  </si>
+  <si>
+    <t>File path of Output Matrix</t>
   </si>
 </sst>
 </file>
@@ -546,7 +555,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -637,7 +646,17 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Add OutputFolderPath to Config.XLSX
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\GitHub\uipath-automation-4\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCFAC4F-F994-400A-A2F7-2564C4B772EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C1B49F-5784-4ACD-8837-B5D7C9437FBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>logF_BusinessProcessName</t>
-  </si>
-  <si>
-    <t>Framework</t>
   </si>
   <si>
     <t>ProcessABCQueue</t>
@@ -176,6 +173,18 @@
   </si>
   <si>
     <t>File path of Output Matrix</t>
+  </si>
+  <si>
+    <t>ProjectPlagiarismBot</t>
+  </si>
+  <si>
+    <t>OutputFolderPath</t>
+  </si>
+  <si>
+    <t>Data\Output</t>
+  </si>
+  <si>
+    <t>Folder path to save Output Matrix</t>
   </si>
 </sst>
 </file>
@@ -555,7 +564,7 @@
   <dimension ref="A1:Z995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -602,13 +611,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -617,47 +626,57 @@
         <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:26" s="5" customFormat="1" ht="14.25" customHeight="1">
       <c r="A7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="C7" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
         <v>47</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>48</v>
       </c>
-      <c r="C8" t="s">
-        <v>49</v>
-      </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1709,7 +1728,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1733,7 +1752,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1755,7 +1774,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1766,7 +1785,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1777,41 +1796,41 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2817,7 +2836,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>